<commit_message>
Se agrega planificación cursos
</commit_message>
<xml_diff>
--- a/Horario.xlsx
+++ b/Horario.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CCGQ095K\Documents\Udemy\udemy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F67CDA97-BD50-47EF-8AEC-E452DE87A370}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9CA49B3-2C67-4060-A247-D0266C0F5E63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cursos" sheetId="2" r:id="rId1"/>
     <sheet name="Step" sheetId="3" r:id="rId2"/>
-    <sheet name="ActividadSemanal" sheetId="1" r:id="rId3"/>
+    <sheet name="Horario Estudio" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,114 +32,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Carlos Garcia Quintupil</author>
-  </authors>
-  <commentList>
-    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{3D86C9FD-99D2-433D-847D-50EA9E065860}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Carlos Garcia Quintupil:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Ver video curso y grabar audio mp3, subir a Drive.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{D42D5471-968E-4986-93C1-134F0A7853B1}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Carlos Garcia Quintupil:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Utilizar IA Wispher para transformar audio a texto y traducir con ChatGpt. Documentar en GitHub.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{D35248CD-0E60-4608-B0CF-ACD3EE28DF74}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Carlos Garcia Quintupil:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Ver video curso</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F3" authorId="0" shapeId="0" xr:uid="{0633B13D-F65C-4A28-A95C-D706F81A88C5}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Carlos Garcia Quintupil:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Explicar lo que se entendio. Escribir pequeñas notas de lo aprendido.</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="57">
   <si>
     <t xml:space="preserve">Hora </t>
   </si>
@@ -162,9 +56,6 @@
     <t>Almuerzo</t>
   </si>
   <si>
-    <t>Total Hora Estudio</t>
-  </si>
-  <si>
     <t>Actividad Semanal</t>
   </si>
   <si>
@@ -198,9 +89,6 @@
     <t>CoffeBreak/preparación daily</t>
   </si>
   <si>
-    <t>Traducir</t>
-  </si>
-  <si>
     <t>Step 01</t>
   </si>
   <si>
@@ -216,9 +104,6 @@
     <t>Step 05</t>
   </si>
   <si>
-    <t xml:space="preserve">Resumir </t>
-  </si>
-  <si>
     <t>Subir a GIT</t>
   </si>
   <si>
@@ -228,15 +113,9 @@
     <t>Codificar</t>
   </si>
   <si>
-    <t>Ver/Registrar</t>
-  </si>
-  <si>
     <t>Probar</t>
   </si>
   <si>
-    <t>Step07</t>
-  </si>
-  <si>
     <t>Step 04</t>
   </si>
   <si>
@@ -258,9 +137,6 @@
     <t>Ver / Entender</t>
   </si>
   <si>
-    <t>Resumir</t>
-  </si>
-  <si>
     <t xml:space="preserve">Configuración </t>
   </si>
   <si>
@@ -270,9 +146,6 @@
     <t>git clone https://github.com/quintupil/udemy.git</t>
   </si>
   <si>
-    <t>Ver/Entender</t>
-  </si>
-  <si>
     <t>Si No Existe Repositorio:</t>
   </si>
   <si>
@@ -328,13 +201,16 @@
   </si>
   <si>
     <t>Si Existe Transcripción:</t>
+  </si>
+  <si>
+    <t>Total Hora Estudio Diario:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -357,45 +233,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
     <font>
       <i/>
@@ -480,7 +317,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -675,11 +512,187 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -689,67 +702,6 @@
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="20" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="20" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="20" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -793,7 +745,7 @@
     <xf numFmtId="0" fontId="2" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -826,6 +778,93 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="11" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="11" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="11" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="11" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="11" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="20" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1106,11 +1145,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15808D90-8F0A-40AC-8DCB-C765D696F850}">
-  <dimension ref="A1:I7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15808D90-8F0A-40AC-8DCB-C765D696F850}">
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1118,124 +1157,117 @@
     <col min="1" max="1" width="54.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="28" t="s">
+      <c r="F1" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" s="28" t="s">
+      <c r="H1" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="28" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="53" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="50">
+        <f>('Horario Estudio'!A5-'Horario Estudio'!A3)+('Horario Estudio'!A7-'Horario Estudio'!A5)+('Horario Estudio'!A9-'Horario Estudio'!A7)+('Horario Estudio'!A11-'Horario Estudio'!A9)</f>
+        <v>8.3333333333333343E-2</v>
+      </c>
+      <c r="C2" s="43"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="44"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="3">
-        <f>(ActividadSemanal!A5-ActividadSemanal!A3)+(ActividadSemanal!A7-ActividadSemanal!A5)+(ActividadSemanal!A9-ActividadSemanal!A7)+(ActividadSemanal!A11-ActividadSemanal!A9)</f>
-        <v>8.3333333333333343E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="B3" s="51">
+        <f>('Horario Estudio'!A13-'Horario Estudio'!A11)+('Horario Estudio'!A15-'Horario Estudio'!A13)+('Horario Estudio'!A17-'Horario Estudio'!A15)</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="C3" s="43"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="45"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2">
-        <f>(ActividadSemanal!A13-ActividadSemanal!A11)+(ActividadSemanal!A15-ActividadSemanal!A13)+(ActividadSemanal!A17-ActividadSemanal!A15)</f>
-        <v>6.25E-2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+      <c r="B4" s="51">
+        <f>('Horario Estudio'!A19-'Horario Estudio'!A17)+('Horario Estudio'!A21-'Horario Estudio'!A19)</f>
+        <v>4.1666666666666685E-2</v>
+      </c>
+      <c r="C4" s="43"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="44"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="2">
-        <f>(ActividadSemanal!A19-ActividadSemanal!A17)+(ActividadSemanal!A21-ActividadSemanal!A19)</f>
-        <v>4.1666666666666685E-2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+      <c r="B5" s="51">
+        <f>('Horario Estudio'!A28-'Horario Estudio'!A26)+('Horario Estudio'!A30-'Horario Estudio'!A28)</f>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="C5" s="43"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="44"/>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="2">
-        <f>(ActividadSemanal!A28-ActividadSemanal!A26)+(ActividadSemanal!A30-ActividadSemanal!A28)</f>
-        <v>4.166666666666663E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="2">
-        <f>(ActividadSemanal!A32-ActividadSemanal!A30)+(ActividadSemanal!A33-ActividadSemanal!A32)</f>
+      <c r="B6" s="52">
+        <f>('Horario Estudio'!A32-'Horario Estudio'!A30)+('Horario Estudio'!A33-'Horario Estudio'!A32)</f>
         <v>3.8194444444444531E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="18" t="str">
+      <c r="C6" s="46"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="49"/>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="37" t="str">
         <f>TEXT(SUM(B2:B6),"[h]:mm:ss")</f>
         <v>6:25:00</v>
       </c>
@@ -1243,7 +1275,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1252,309 +1283,309 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.28515625" style="31" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58" style="31" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="72.42578125" style="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" style="31" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" style="31" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="43.85546875" style="31" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="11.42578125" style="31"/>
+    <col min="1" max="1" width="47.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="72.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="11.42578125" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="D2" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="31" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="50" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" s="50" t="s">
-        <v>56</v>
-      </c>
-      <c r="E1" s="50" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" s="51" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="52" t="s">
-        <v>59</v>
-      </c>
-      <c r="B2" s="53" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" s="54" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" s="55" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="55" t="s">
+      <c r="F3" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="56" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="40" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="D3" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="E3" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="F3" s="40" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="43" t="str">
+      <c r="A4" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="16"/>
+      <c r="C4" s="18" t="str">
         <f>TEXT("-&gt;estudiarTranscripcion();","")</f>
         <v>-&gt;estudiarTranscripcion();</v>
       </c>
-      <c r="D4" s="32"/>
-      <c r="E4" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="F4" s="41" t="s">
-        <v>52</v>
+      <c r="D4" s="7"/>
+      <c r="E4" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="39" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5" s="35" t="str">
+      <c r="A5" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="10" t="str">
         <f>TEXT("-&gt;descargarMp3ToFolderCourse();","")</f>
         <v>-&gt;descargarMp3ToFolderCourse();</v>
       </c>
-      <c r="C5" s="35" t="str">
+      <c r="C5" s="10" t="str">
         <f>TEXT("-&gt;destacarTranscripcion();","")</f>
         <v>-&gt;destacarTranscripcion();</v>
       </c>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="41" t="s">
-        <v>36</v>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="16" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="34" t="str">
+      <c r="A6" s="9" t="str">
         <f>TEXT("-&gt; CreateFolderCourse();","")</f>
         <v>-&gt; CreateFolderCourse();</v>
       </c>
-      <c r="B6" s="35" t="str">
+      <c r="B6" s="10" t="str">
         <f>TEXT("-&gt;configurarIAWispherInGoogleColab();","")</f>
         <v>-&gt;configurarIAWispherInGoogleColab();</v>
       </c>
-      <c r="C6" s="41" t="s">
-        <v>57</v>
-      </c>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
+      <c r="C6" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="39" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" s="35" t="str">
+      <c r="A7" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="10" t="str">
         <f>TEXT("-&gt;subirMp3ToGoogleColab();","")</f>
         <v>-&gt;subirMp3ToGoogleColab();</v>
       </c>
-      <c r="C7" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
+      <c r="C7" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="44" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" s="35" t="str">
+      <c r="A8" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="10" t="str">
         <f>TEXT("-&gt;ejecutarIAWispher();","")</f>
         <v>-&gt;ejecutarIAWispher();</v>
       </c>
-      <c r="C8" s="35" t="str">
+      <c r="C8" s="10" t="str">
         <f>TEXT("-&gt; documentarLoAprendido();","")</f>
         <v>-&gt; documentarLoAprendido();</v>
       </c>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="B9" s="35" t="str">
+      <c r="A9" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="10" t="str">
         <f>TEXT("-&gt;descargarTranscripcionGoogleColab();","")</f>
         <v>-&gt;descargarTranscripcionGoogleColab();</v>
       </c>
-      <c r="C9" s="41" t="s">
-        <v>58</v>
-      </c>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
+      <c r="C9" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="34" t="str">
+      <c r="A10" s="9" t="str">
         <f>TEXT("-&gt;iniciarGrabacionCelular();", "")</f>
         <v>-&gt;iniciarGrabacionCelular();</v>
       </c>
-      <c r="B10" s="35" t="str">
+      <c r="B10" s="10" t="str">
         <f>TEXT("-&gt;moverTranscripcionFolderCourse();","")</f>
         <v>-&gt;moverTranscripcionFolderCourse();</v>
       </c>
-      <c r="C10" s="41" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
+      <c r="C10" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="34" t="str">
+      <c r="A11" s="9" t="str">
         <f>TEXT("-&gt;verVideoCurso();","")</f>
         <v>-&gt;verVideoCurso();</v>
       </c>
-      <c r="B11" s="41" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" s="35"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
+      <c r="B11" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="10"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
     </row>
     <row r="12" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="34" t="str">
+      <c r="A12" s="9" t="str">
         <f>TEXT("-&gt;subirMp3HaciaDriveGoogle();","")</f>
         <v>-&gt;subirMp3HaciaDriveGoogle();</v>
       </c>
-      <c r="B12" s="41" t="s">
-        <v>60</v>
-      </c>
-      <c r="C12" s="37"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="32"/>
+      <c r="B12" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="12"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="7"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="35" t="str">
+      <c r="B13" s="10" t="str">
         <f>TEXT("-&gt;chatGptTraducirAEspañolTranscipcion();","")</f>
         <v>-&gt;chatGptTraducirAEspañolTranscipcion();</v>
       </c>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="33"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="8"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="35" t="str">
+      <c r="B14" s="10" t="str">
         <f>TEXT("-&gt;documentarTranscripcion();","")</f>
         <v>-&gt;documentarTranscripcion();</v>
       </c>
-      <c r="C14" s="33"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="32"/>
-      <c r="B15" s="48" t="s">
-        <v>61</v>
-      </c>
-      <c r="C15" s="32"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
+      <c r="A15" s="7"/>
+      <c r="B15" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="29"/>
-      <c r="B16" s="43" t="str">
+      <c r="A16" s="4"/>
+      <c r="B16" s="18" t="str">
         <f>TEXT("-&gt;documentarTranscripcion();","")</f>
         <v>-&gt;documentarTranscripcion();</v>
       </c>
-      <c r="C16" s="42"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="36"/>
-      <c r="B17" s="46" t="s">
-        <v>48</v>
-      </c>
-      <c r="C17" s="47"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
+      <c r="A17" s="11"/>
+      <c r="B17" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="22"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="30"/>
-      <c r="B18" s="30"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="30"/>
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="30"/>
-      <c r="B19" s="30"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="30"/>
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="30"/>
-      <c r="B20" s="30"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="30"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="30"/>
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="30"/>
-      <c r="B21" s="30"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="30"/>
-      <c r="B22" s="30"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="30"/>
-      <c r="F22" s="30"/>
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1566,8 +1597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1579,287 +1610,287 @@
     <col min="5" max="5" width="48.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>8</v>
+      <c r="B1" s="28" t="s">
+        <v>7</v>
       </c>
       <c r="D1"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="A2" s="33">
         <v>0.20833333333333334</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="63" t="s">
         <v>1</v>
       </c>
       <c r="D2"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="13">
+      <c r="A3" s="55">
         <v>0.22916666666666666</v>
       </c>
-      <c r="B3" s="4" t="str">
+      <c r="B3" s="35" t="str">
         <f>Cursos!A2</f>
         <v>Wall Street English</v>
       </c>
       <c r="D3"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="A4" s="33">
         <v>0.24652777777777779</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="63" t="s">
         <v>2</v>
       </c>
       <c r="D4"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="13">
+      <c r="A5" s="55">
         <v>0.25</v>
       </c>
-      <c r="B5" s="4" t="str">
+      <c r="B5" s="35" t="str">
         <f>Cursos!A2</f>
         <v>Wall Street English</v>
       </c>
       <c r="D5"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="33">
         <v>0.2673611111111111</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="63" t="s">
         <v>2</v>
       </c>
       <c r="D6"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="13">
+      <c r="A7" s="55">
         <v>0.27083333333333331</v>
       </c>
-      <c r="B7" s="4" t="str">
+      <c r="B7" s="35" t="str">
         <f>Cursos!A2</f>
         <v>Wall Street English</v>
       </c>
       <c r="D7"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="A8" s="33">
         <v>0.28819444444444448</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="63" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="13">
+      <c r="A9" s="55">
         <v>0.29166666666666669</v>
       </c>
-      <c r="B9" s="5" t="str">
+      <c r="B9" s="64" t="str">
         <f>Cursos!A2</f>
         <v>Wall Street English</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+      <c r="A10" s="33">
         <v>0.30902777777777779</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="63" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="14">
+      <c r="A11" s="56">
         <v>0.3125</v>
       </c>
-      <c r="B11" s="6" t="str">
+      <c r="B11" s="65" t="str">
         <f>Cursos!A3</f>
         <v>The Complete 2023 Web Development</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+      <c r="A12" s="33">
         <v>0.3298611111111111</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="63" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="14">
+      <c r="A13" s="56">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B13" s="6" t="str">
+      <c r="B13" s="65" t="str">
         <f>Cursos!A3</f>
         <v>The Complete 2023 Web Development</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
+      <c r="A14" s="33">
         <v>0.35069444444444442</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="63" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="14">
+      <c r="A15" s="56">
         <v>0.35416666666666669</v>
       </c>
-      <c r="B15" s="6" t="str">
+      <c r="B15" s="65" t="str">
         <f>Cursos!A3</f>
         <v>The Complete 2023 Web Development</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="25">
+      <c r="A16" s="57">
         <v>0.37152777777777773</v>
       </c>
-      <c r="B16" s="24" t="s">
-        <v>14</v>
+      <c r="B16" s="66" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="15">
+      <c r="A17" s="58">
         <v>0.375</v>
       </c>
-      <c r="B17" s="7" t="str">
+      <c r="B17" s="67" t="str">
         <f>Cursos!A4</f>
         <v>Master en CSS: Responsive, SAAS, Flexbox, Grid y Bootstrap</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
+      <c r="A18" s="33">
         <v>0.3923611111111111</v>
       </c>
-      <c r="B18" t="s">
-        <v>17</v>
+      <c r="B18" s="63" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="15">
+      <c r="A19" s="58">
         <v>0.39583333333333331</v>
       </c>
-      <c r="B19" s="7" t="str">
+      <c r="B19" s="67" t="str">
         <f>Cursos!A4</f>
         <v>Master en CSS: Responsive, SAAS, Flexbox, Grid y Bootstrap</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
+      <c r="A20" s="33">
         <v>0.41319444444444442</v>
       </c>
-      <c r="B20" t="s">
-        <v>18</v>
+      <c r="B20" s="63" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="25">
+      <c r="A21" s="57">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B21" s="24" t="s">
+      <c r="B21" s="66" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
+      <c r="A22" s="33">
         <v>0.4381944444444445</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="63" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="59">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="B23" s="68" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="33">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="B24" s="63" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="57">
+        <v>0.75</v>
+      </c>
+      <c r="B25" s="66" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="26">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="B23" s="27" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="B24" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="25">
-        <v>0.75</v>
-      </c>
-      <c r="B25" s="24" t="s">
-        <v>16</v>
-      </c>
-    </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="16">
+      <c r="A26" s="60">
         <v>0.83333333333333337</v>
       </c>
-      <c r="B26" s="11" t="str">
+      <c r="B26" s="69" t="str">
         <f>Cursos!A5</f>
         <v>JavaScript Moderno: Guía para dominar el lenguaje</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
+      <c r="A27" s="33">
         <v>0.85069444444444453</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="63" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="16">
+      <c r="A28" s="60">
         <v>0.85416666666666663</v>
       </c>
-      <c r="B28" s="11" t="str">
+      <c r="B28" s="69" t="str">
         <f>Cursos!A5</f>
         <v>JavaScript Moderno: Guía para dominar el lenguaje</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="3">
+      <c r="A29" s="33">
         <v>0.87152777777777779</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="63" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="17">
+      <c r="A30" s="61">
         <v>0.875</v>
       </c>
-      <c r="B30" s="12" t="str">
+      <c r="B30" s="70" t="str">
         <f>Cursos!A6</f>
         <v xml:space="preserve">Curso Git + GitHub </v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="3">
+      <c r="A31" s="33">
         <v>0.89236111111111116</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="63" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="17">
+      <c r="A32" s="61">
         <v>0.89583333333333337</v>
       </c>
-      <c r="B32" s="12" t="str">
+      <c r="B32" s="70" t="str">
         <f>Cursos!A6</f>
         <v xml:space="preserve">Curso Git + GitHub </v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="3">
+    <row r="33" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="62">
         <v>0.91319444444444453</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="71" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>